<commit_message>
Improved docs, updated bom
</commit_message>
<xml_diff>
--- a/files/bom.xlsx
+++ b/files/bom.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,9 @@
     <t>ADXL345</t>
   </si>
   <si>
+    <t>5V step down</t>
+  </si>
+  <si>
     <t>Motion</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>90deg side mount</t>
+  </si>
+  <si>
+    <t>20pcs</t>
   </si>
   <si>
     <t>2020 I-Type Nut 5 - 800mm</t>
@@ -818,6 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -885,8 +892,8 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="8">
-        <f>SUM(G3:G4)</f>
-        <v>7.46</v>
+        <f>SUM(G3:G5)</f>
+        <v>10.85</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -925,7 +932,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="13">
-        <f t="shared" ref="G3:G4" si="1">MULTIPLY(B3, C3)</f>
+        <f t="shared" ref="G3:G5" si="1">MULTIPLY(B3, C3)</f>
         <v>5.67</v>
       </c>
     </row>
@@ -948,325 +955,336 @@
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>3.39</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="1"/>
+        <v>3.39</v>
+      </c>
     </row>
     <row r="6">
       <c r="C6" s="13"/>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" ht="18.0" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="8">
-        <f>SUM(G8:G19)</f>
+    <row r="7">
+      <c r="C7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" ht="18.0" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="8">
+        <f>SUM(G9:G20)</f>
         <v>37.75</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10">
         <v>1.0</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C9" s="11">
         <v>1.29</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="13">
-        <f>MULTIPLY(B8, C8)</f>
+      <c r="E9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="13">
+        <f>MULTIPLY(B9, C9)</f>
         <v>1.29</v>
       </c>
     </row>
-    <row r="9">
-      <c r="C9" s="11"/>
-      <c r="G9" s="13"/>
-    </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C10" s="11">
-        <v>5.59</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="13">
-        <f t="shared" ref="G10:G11" si="2">MULTIPLY(B10, C10)</f>
-        <v>11.18</v>
-      </c>
+      <c r="C10" s="11"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" s="11">
-        <v>1.69</v>
+        <v>5.59</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" ref="G11:G12" si="2">MULTIPLY(B11, C11)</f>
+        <v>11.18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="13">
+      <c r="B12" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1.69</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="13">
         <f t="shared" si="2"/>
         <v>6.76</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="G12" s="13"/>
-    </row>
     <row r="13">
-      <c r="A13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="C13" s="11">
-        <v>1.65</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="13">
-        <f t="shared" ref="G13:G14" si="3">MULTIPLY(B13, C13)</f>
-        <v>6.6</v>
-      </c>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C14" s="11">
-        <v>2.84</v>
+        <v>1.65</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" ref="G14:G15" si="3">MULTIPLY(B14, C14)</f>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="13">
+      <c r="B15" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>2.84</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="13">
         <f t="shared" si="3"/>
         <v>2.84</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="G15" s="13"/>
-    </row>
     <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="10">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="10">
         <v>1.0</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C17" s="11">
         <v>2.85</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="13">
-        <f>MULTIPLY(B16, C16)</f>
+      <c r="E17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="13">
+        <f>MULTIPLY(B17, C17)</f>
         <v>2.85</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="G17" s="13"/>
-    </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C18" s="11">
-        <v>2.09</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="13">
-        <f t="shared" ref="G18:G19" si="4">MULTIPLY(B18, C18)</f>
-        <v>4.18</v>
-      </c>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C19" s="11">
-        <v>2.05</v>
+        <v>2.09</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="13">
+        <f t="shared" ref="G19:G20" si="4">MULTIPLY(B19, C19)</f>
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="13">
+      <c r="B20" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2.05</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="13">
         <f t="shared" si="4"/>
         <v>2.05</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="13"/>
-      <c r="G20" s="13"/>
     </row>
     <row r="21">
       <c r="C21" s="13"/>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" ht="18.0" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="8">
-        <f>SUM(G23:G24)</f>
+    <row r="22">
+      <c r="C22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" ht="18.0" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="8">
+        <f>SUM(G24:G25)</f>
         <v>8.76</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C23" s="11">
-        <v>1.69</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="13">
-        <f t="shared" ref="G23:G24" si="5">MULTIPLY(B23, C23)</f>
-        <v>3.38</v>
-      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="10">
         <v>2.0</v>
       </c>
       <c r="C24" s="11">
-        <v>2.69</v>
+        <v>1.69</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="13">
+        <f t="shared" ref="G24:G25" si="5">MULTIPLY(B24, C24)</f>
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="13">
+      <c r="B25" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C25" s="11">
+        <v>2.69</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="13">
         <f t="shared" si="5"/>
         <v>5.38</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="10"/>
-      <c r="G25" s="11"/>
     </row>
     <row r="26">
       <c r="A26" s="10"/>
@@ -1275,81 +1293,70 @@
       <c r="D26" s="10"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" ht="18.0" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="8">
-        <f>SUM(G28:G43)</f>
-        <v>85.72</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="10" t="s">
+    <row r="27">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="10"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" ht="18.0" customHeight="1">
+      <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C28" s="11">
-        <v>2.59</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="8">
+        <f>SUM(G29:G44)</f>
+        <v>85.73</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C29" s="11">
+        <v>5.19</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="13">
-        <f>MULTIPLY(B28, C28)</f>
-        <v>5.18</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="E29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="13">
+        <f>MULTIPLY(B29, C29)</f>
+        <v>5.19</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C30" s="11">
-        <v>6.02</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="13">
-        <f t="shared" ref="G30:G40" si="6">MULTIPLY(B30, C30)</f>
-        <v>12.04</v>
-      </c>
+      <c r="C30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
@@ -1359,53 +1366,50 @@
         <v>2.0</v>
       </c>
       <c r="C31" s="11">
+        <v>6.02</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="13">
+        <f t="shared" ref="G31:G41" si="6">MULTIPLY(B31, C31)</f>
+        <v>12.04</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C32" s="11">
         <v>3.11</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" s="13">
+      <c r="D32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="13">
         <f t="shared" si="6"/>
         <v>6.22</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="10" t="s">
+    <row r="33">
+      <c r="A33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C33" s="11">
+        <v>5.52</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C32" s="11">
-        <v>5.52</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="13">
+      <c r="G33" s="13">
         <f t="shared" si="6"/>
         <v>5.52</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C33" s="11">
-        <v>2.94</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="13">
-        <f t="shared" si="6"/>
-        <v>5.88</v>
       </c>
     </row>
     <row r="34">
@@ -1416,17 +1420,17 @@
         <v>2.0</v>
       </c>
       <c r="C34" s="11">
-        <v>3.38</v>
+        <v>2.94</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>42</v>
       </c>
       <c r="G34" s="13">
         <f t="shared" si="6"/>
-        <v>6.76</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="35">
@@ -1434,45 +1438,41 @@
         <v>43</v>
       </c>
       <c r="B35" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C35" s="11">
-        <v>2.46</v>
+        <v>3.38</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G35" s="13">
         <f t="shared" si="6"/>
-        <v>9.84</v>
-      </c>
-      <c r="H35" s="13"/>
+        <v>6.76</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C36" s="11">
+        <v>2.46</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="B36" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="C36" s="11">
-        <v>1.23</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="G36" s="13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>9.84</v>
       </c>
       <c r="H36" s="13"/>
     </row>
@@ -1481,65 +1481,66 @@
         <v>46</v>
       </c>
       <c r="B37" s="10">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="C37" s="11">
-        <v>2.44</v>
+        <v>1.23</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="G37" s="13">
         <f t="shared" si="6"/>
-        <v>4.88</v>
+        <v>0</v>
       </c>
       <c r="H37" s="13"/>
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38" s="10">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C38" s="11">
-        <v>1.12</v>
+        <v>2.44</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G38" s="13">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+        <v>4.88</v>
+      </c>
+      <c r="H38" s="13"/>
     </row>
     <row r="39">
       <c r="A39" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" s="10">
         <v>0.0</v>
       </c>
       <c r="C39" s="11">
-        <v>0.98</v>
+        <v>1.12</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G39" s="13">
         <f t="shared" si="6"/>
@@ -1548,272 +1549,275 @@
     </row>
     <row r="40">
       <c r="A40" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" s="10">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C40" s="11">
-        <v>2.78</v>
+        <v>0.98</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="G40" s="13">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C41" s="11">
         <v>2.78</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="C41" s="13"/>
-      <c r="G41" s="13"/>
+      <c r="D41" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="13">
+        <f t="shared" si="6"/>
+        <v>2.78</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C42" s="11">
-        <v>4.54</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" s="13">
-        <f t="shared" ref="G42:G43" si="7">MULTIPLY(B42, C42)</f>
-        <v>9.08</v>
-      </c>
+      <c r="C42" s="13"/>
+      <c r="G42" s="13"/>
     </row>
     <row r="43">
       <c r="A43" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B43" s="10">
         <v>2.0</v>
       </c>
       <c r="C43" s="11">
+        <v>4.54</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="13">
+        <f t="shared" ref="G43:G44" si="7">MULTIPLY(B43, C43)</f>
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C44" s="11">
         <v>8.77</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="13">
+      <c r="D44" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" s="13">
         <f t="shared" si="7"/>
         <v>17.54</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="C44" s="13"/>
-      <c r="G44" s="13"/>
     </row>
     <row r="45">
       <c r="C45" s="13"/>
       <c r="G45" s="13"/>
     </row>
-    <row r="46" ht="18.0" customHeight="1">
-      <c r="A46" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="8">
-        <f>SUM(G47:G51)</f>
+    <row r="46">
+      <c r="C46" s="13"/>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" ht="18.0" customHeight="1">
+      <c r="A47" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="8">
+        <f>SUM(G48:G52)</f>
         <v>17.95</v>
       </c>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="9"/>
-      <c r="Z46" s="9"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C47" s="11">
-        <v>8.53</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G47" s="13">
-        <f t="shared" ref="G47:G51" si="8">MULTIPLY(B47, C47)</f>
-        <v>8.53</v>
-      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="9"/>
     </row>
     <row r="48">
       <c r="A48" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="10">
         <v>1.0</v>
       </c>
       <c r="C48" s="11">
-        <v>2.05</v>
+        <v>8.53</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G48" s="13">
+        <f t="shared" ref="G48:G52" si="8">MULTIPLY(B48, C48)</f>
+        <v>8.53</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C49" s="11">
+        <v>2.05</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" s="13">
         <f t="shared" si="8"/>
         <v>2.05</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="10" t="s">
+    <row r="50">
+      <c r="A50" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C50" s="11">
+        <v>4.17</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C49" s="11">
-        <v>4.17</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G49" s="13">
+      <c r="E50" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G50" s="13">
         <f t="shared" si="8"/>
         <v>4.17</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="10" t="s">
+    <row r="51">
+      <c r="A51" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C51" s="11">
+        <v>1.76</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C50" s="11">
-        <v>1.76</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G50" s="13">
+      <c r="E51" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="13">
         <f t="shared" si="8"/>
         <v>1.76</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="10" t="s">
+    <row r="52">
+      <c r="A52" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C52" s="11">
+        <v>1.44</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C51" s="11">
-        <v>1.44</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G51" s="13">
+      <c r="E52" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" s="13">
         <f t="shared" si="8"/>
         <v>1.44</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="C52" s="13"/>
-      <c r="G52" s="13"/>
     </row>
     <row r="53">
       <c r="C53" s="13"/>
       <c r="G53" s="13"/>
     </row>
-    <row r="54" ht="18.0" customHeight="1">
-      <c r="A54" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="6"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="8">
-        <f>SUM(G55:G72)</f>
+    <row r="54">
+      <c r="C54" s="13"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" ht="18.0" customHeight="1">
+      <c r="A55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="8">
+        <f>SUM(G56:G73)</f>
         <v>38.42</v>
       </c>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="9"/>
-      <c r="Z54" s="9"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C55" s="11">
-        <v>2.79</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G55" s="13">
-        <f t="shared" ref="G55:G56" si="9">MULTIPLY(B55, C55)</f>
-        <v>2.79</v>
-      </c>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="9"/>
+      <c r="Z55" s="9"/>
     </row>
     <row r="56">
       <c r="A56" s="10" t="s">
@@ -1823,7 +1827,7 @@
         <v>1.0</v>
       </c>
       <c r="C56" s="11">
-        <v>3.09</v>
+        <v>2.79</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>8</v>
@@ -1832,73 +1836,73 @@
         <v>65</v>
       </c>
       <c r="G56" s="13">
+        <f t="shared" ref="G56:G57" si="9">MULTIPLY(B56, C56)</f>
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C57" s="11">
+        <v>3.09</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G57" s="13">
         <f t="shared" si="9"/>
         <v>3.09</v>
       </c>
     </row>
-    <row r="57">
-      <c r="C57" s="13"/>
-      <c r="G57" s="13"/>
-    </row>
     <row r="58">
-      <c r="A58" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" s="10">
+      <c r="C58" s="13"/>
+      <c r="G58" s="13"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="10">
         <v>1.0</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C59" s="11">
         <v>2.05</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D59" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G58" s="13">
-        <f>MULTIPLY(B58, C58)</f>
+      <c r="E59" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" s="13">
+        <f>MULTIPLY(B59, C59)</f>
         <v>2.05</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="10"/>
-      <c r="G59" s="13"/>
-    </row>
     <row r="60">
-      <c r="A60" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C60" s="11">
-        <v>1.9</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G60" s="13">
-        <f t="shared" ref="G60:G69" si="10">MULTIPLY(B60, C60)</f>
-        <v>3.8</v>
-      </c>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="10"/>
+      <c r="G60" s="13"/>
     </row>
     <row r="61">
       <c r="A61" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B61" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C61" s="11">
-        <v>2.06</v>
+        <v>1.9</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>8</v>
@@ -1907,8 +1911,8 @@
         <v>71</v>
       </c>
       <c r="G61" s="13">
-        <f t="shared" si="10"/>
-        <v>2.06</v>
+        <f t="shared" ref="G61:G70" si="10">MULTIPLY(B61, C61)</f>
+        <v>3.8</v>
       </c>
     </row>
     <row r="62">
@@ -1916,10 +1920,10 @@
         <v>72</v>
       </c>
       <c r="B62" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C62" s="11">
-        <v>1.83</v>
+        <v>2.06</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>8</v>
@@ -1929,7 +1933,7 @@
       </c>
       <c r="G62" s="13">
         <f t="shared" si="10"/>
-        <v>3.66</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="63">
@@ -1937,10 +1941,10 @@
         <v>74</v>
       </c>
       <c r="B63" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C63" s="11">
-        <v>1.98</v>
+        <v>1.83</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>8</v>
@@ -1950,7 +1954,7 @@
       </c>
       <c r="G63" s="13">
         <f t="shared" si="10"/>
-        <v>1.98</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="64">
@@ -1958,10 +1962,10 @@
         <v>76</v>
       </c>
       <c r="B64" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C64" s="11">
-        <v>1.72</v>
+        <v>1.98</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>8</v>
@@ -1971,7 +1975,7 @@
       </c>
       <c r="G64" s="13">
         <f t="shared" si="10"/>
-        <v>3.44</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="65">
@@ -1979,10 +1983,10 @@
         <v>78</v>
       </c>
       <c r="B65" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C65" s="11">
-        <v>2.23</v>
+        <v>1.72</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>8</v>
@@ -1992,7 +1996,7 @@
       </c>
       <c r="G65" s="13">
         <f t="shared" si="10"/>
-        <v>2.23</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="66">
@@ -2003,7 +2007,7 @@
         <v>1.0</v>
       </c>
       <c r="C66" s="11">
-        <v>1.61</v>
+        <v>2.23</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>8</v>
@@ -2013,7 +2017,7 @@
       </c>
       <c r="G66" s="13">
         <f t="shared" si="10"/>
-        <v>1.61</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="67">
@@ -2024,7 +2028,7 @@
         <v>1.0</v>
       </c>
       <c r="C67" s="11">
-        <v>3.35</v>
+        <v>1.61</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>8</v>
@@ -2034,7 +2038,7 @@
       </c>
       <c r="G67" s="13">
         <f t="shared" si="10"/>
-        <v>3.35</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="68">
@@ -2045,7 +2049,7 @@
         <v>1.0</v>
       </c>
       <c r="C68" s="11">
-        <v>1.49</v>
+        <v>3.35</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>8</v>
@@ -2055,7 +2059,7 @@
       </c>
       <c r="G68" s="13">
         <f t="shared" si="10"/>
-        <v>1.49</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="69">
@@ -2066,7 +2070,7 @@
         <v>1.0</v>
       </c>
       <c r="C69" s="11">
-        <v>1.45</v>
+        <v>1.49</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>8</v>
@@ -2076,37 +2080,37 @@
       </c>
       <c r="G69" s="13">
         <f t="shared" si="10"/>
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C70" s="11">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="10"/>
-      <c r="G70" s="13"/>
+      <c r="D70" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G70" s="13">
+        <f t="shared" si="10"/>
+        <v>1.45</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C71" s="11">
-        <v>3.19</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="G71" s="13">
-        <f t="shared" ref="G71:G72" si="11">MULTIPLY(B71, C71)</f>
-        <v>3.19</v>
-      </c>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="10"/>
+      <c r="G71" s="13"/>
     </row>
     <row r="72">
       <c r="A72" s="10" t="s">
@@ -2116,7 +2120,7 @@
         <v>1.0</v>
       </c>
       <c r="C72" s="11">
-        <v>2.23</v>
+        <v>3.19</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>8</v>
@@ -2125,136 +2129,153 @@
         <v>91</v>
       </c>
       <c r="G72" s="13">
+        <f t="shared" ref="G72:G73" si="11">MULTIPLY(B72, C72)</f>
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C73" s="11">
+        <v>2.23</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G73" s="13">
         <f t="shared" si="11"/>
         <v>2.23</v>
       </c>
-    </row>
-    <row r="73">
-      <c r="C73" s="13"/>
-      <c r="G73" s="13"/>
     </row>
     <row r="74">
       <c r="C74" s="13"/>
       <c r="G74" s="13"/>
     </row>
-    <row r="75" ht="18.0" customHeight="1">
-      <c r="A75" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B75" s="6"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="8">
-        <f>SUM(G76:G78)</f>
+    <row r="75">
+      <c r="C75" s="13"/>
+      <c r="G75" s="13"/>
+    </row>
+    <row r="76" ht="18.0" customHeight="1">
+      <c r="A76" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="8">
+        <f>SUM(G77:G79)</f>
         <v>9.9</v>
       </c>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-      <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
-      <c r="R75" s="9"/>
-      <c r="S75" s="9"/>
-      <c r="T75" s="9"/>
-      <c r="U75" s="9"/>
-      <c r="V75" s="9"/>
-      <c r="W75" s="9"/>
-      <c r="X75" s="9"/>
-      <c r="Y75" s="9"/>
-      <c r="Z75" s="9"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B76" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C76" s="11">
-        <v>-6.0</v>
-      </c>
-      <c r="G76" s="13">
-        <f t="shared" ref="G76:G78" si="12">MULTIPLY(B76, C76)</f>
-        <v>-6</v>
-      </c>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="9"/>
+      <c r="R76" s="9"/>
+      <c r="S76" s="9"/>
+      <c r="T76" s="9"/>
+      <c r="U76" s="9"/>
+      <c r="V76" s="9"/>
+      <c r="W76" s="9"/>
+      <c r="X76" s="9"/>
+      <c r="Y76" s="9"/>
+      <c r="Z76" s="9"/>
     </row>
     <row r="77">
       <c r="A77" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B77" s="10">
         <v>1.0</v>
       </c>
       <c r="C77" s="11">
+        <v>-6.0</v>
+      </c>
+      <c r="G77" s="13">
+        <f t="shared" ref="G77:G79" si="12">MULTIPLY(B77, C77)</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C78" s="11">
         <v>5.95</v>
       </c>
-      <c r="G77" s="13">
+      <c r="G78" s="13">
         <f t="shared" si="12"/>
         <v>5.95</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B78" s="10">
+    <row r="79">
+      <c r="A79" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" s="10">
         <v>1.0</v>
       </c>
-      <c r="C78" s="11">
+      <c r="C79" s="11">
         <v>9.95</v>
       </c>
-      <c r="G78" s="13">
+      <c r="G79" s="13">
         <f t="shared" si="12"/>
         <v>9.95</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="11"/>
-      <c r="G79" s="13"/>
-    </row>
     <row r="80">
-      <c r="C80" s="13"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="11"/>
       <c r="G80" s="13"/>
     </row>
     <row r="81">
       <c r="C81" s="13"/>
-      <c r="F81" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G81" s="16">
-        <f>SUM(G22, G27, G7, G46,G2, G75, G54)</f>
-        <v>205.96</v>
-      </c>
+      <c r="G81" s="13"/>
     </row>
     <row r="82">
       <c r="C82" s="13"/>
-      <c r="F82" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G82" s="18">
-        <f>SUM(G81,94.98)</f>
-        <v>300.94</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="I82" s="20">
-        <f>MULTIPLY(G82,1.09)</f>
-        <v>328.0246</v>
+      <c r="F82" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" s="16">
+        <f>SUM(G23, G28, G8, G47,G2, G76, G55)</f>
+        <v>209.36</v>
       </c>
     </row>
     <row r="83">
       <c r="C83" s="13"/>
-      <c r="G83" s="13"/>
+      <c r="F83" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G83" s="18">
+        <f>SUM(G82,94.98)</f>
+        <v>304.34</v>
+      </c>
+      <c r="H83" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I83" s="20">
+        <f>MULTIPLY(G83,1.09)</f>
+        <v>331.7306</v>
+      </c>
     </row>
     <row r="84">
       <c r="C84" s="13"/>
@@ -2266,11 +2287,11 @@
     </row>
     <row r="86">
       <c r="C86" s="13"/>
-      <c r="G86" s="11"/>
+      <c r="G86" s="13"/>
     </row>
     <row r="87">
       <c r="C87" s="13"/>
-      <c r="G87" s="13"/>
+      <c r="G87" s="11"/>
     </row>
     <row r="88">
       <c r="C88" s="13"/>
@@ -6159,23 +6180,27 @@
     <row r="1059">
       <c r="C1059" s="13"/>
       <c r="G1059" s="13"/>
+    </row>
+    <row r="1060">
+      <c r="C1060" s="13"/>
+      <c r="G1060" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="D3"/>
     <hyperlink r:id="rId2" ref="D4"/>
-    <hyperlink r:id="rId3" ref="D8"/>
-    <hyperlink r:id="rId4" ref="D10"/>
+    <hyperlink r:id="rId3" ref="D5"/>
+    <hyperlink r:id="rId4" ref="D9"/>
     <hyperlink r:id="rId5" ref="D11"/>
-    <hyperlink r:id="rId6" ref="D13"/>
+    <hyperlink r:id="rId6" ref="D12"/>
     <hyperlink r:id="rId7" ref="D14"/>
-    <hyperlink r:id="rId8" ref="D16"/>
-    <hyperlink r:id="rId9" ref="D18"/>
+    <hyperlink r:id="rId8" ref="D15"/>
+    <hyperlink r:id="rId9" ref="D17"/>
     <hyperlink r:id="rId10" ref="D19"/>
-    <hyperlink r:id="rId11" ref="D23"/>
+    <hyperlink r:id="rId11" ref="D20"/>
     <hyperlink r:id="rId12" ref="D24"/>
-    <hyperlink r:id="rId13" ref="D28"/>
-    <hyperlink r:id="rId14" ref="D30"/>
+    <hyperlink r:id="rId13" ref="D25"/>
+    <hyperlink r:id="rId14" ref="D29"/>
     <hyperlink r:id="rId15" ref="D31"/>
     <hyperlink r:id="rId16" ref="D32"/>
     <hyperlink r:id="rId17" ref="D33"/>
@@ -6186,17 +6211,17 @@
     <hyperlink r:id="rId22" ref="D38"/>
     <hyperlink r:id="rId23" ref="D39"/>
     <hyperlink r:id="rId24" ref="D40"/>
-    <hyperlink r:id="rId25" ref="D42"/>
+    <hyperlink r:id="rId25" ref="D41"/>
     <hyperlink r:id="rId26" ref="D43"/>
-    <hyperlink r:id="rId27" ref="D47"/>
+    <hyperlink r:id="rId27" ref="D44"/>
     <hyperlink r:id="rId28" ref="D48"/>
     <hyperlink r:id="rId29" ref="D49"/>
     <hyperlink r:id="rId30" ref="D50"/>
     <hyperlink r:id="rId31" ref="D51"/>
-    <hyperlink r:id="rId32" ref="D55"/>
+    <hyperlink r:id="rId32" ref="D52"/>
     <hyperlink r:id="rId33" ref="D56"/>
-    <hyperlink r:id="rId34" ref="D58"/>
-    <hyperlink r:id="rId35" ref="D60"/>
+    <hyperlink r:id="rId34" ref="D57"/>
+    <hyperlink r:id="rId35" ref="D59"/>
     <hyperlink r:id="rId36" ref="D61"/>
     <hyperlink r:id="rId37" ref="D62"/>
     <hyperlink r:id="rId38" ref="D63"/>
@@ -6206,10 +6231,14 @@
     <hyperlink r:id="rId42" ref="D67"/>
     <hyperlink r:id="rId43" ref="D68"/>
     <hyperlink r:id="rId44" ref="D69"/>
-    <hyperlink r:id="rId45" ref="D71"/>
+    <hyperlink r:id="rId45" ref="D70"/>
     <hyperlink r:id="rId46" ref="D72"/>
+    <hyperlink r:id="rId47" ref="D73"/>
   </hyperlinks>
-  <drawing r:id="rId47"/>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <drawing r:id="rId48"/>
 </worksheet>
 </file>
 
@@ -6309,7 +6338,7 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B3" s="10">
         <v>1.0</v>
@@ -6321,10 +6350,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G3" s="13">
         <f t="shared" ref="G3:G6" si="1">MULTIPLY(B3, C3)</f>
@@ -6333,7 +6362,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B4" s="10">
         <v>2.0</v>
@@ -6342,10 +6371,10 @@
         <v>22.29</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G4" s="13">
         <f t="shared" si="1"/>
@@ -6354,7 +6383,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B5" s="10">
         <v>0.0</v>
@@ -6366,10 +6395,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="1"/>
@@ -6378,7 +6407,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B6" s="10">
         <v>1.0</v>
@@ -6390,10 +6419,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="1"/>
@@ -6406,7 +6435,7 @@
     </row>
     <row r="8" ht="18.0" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -6439,7 +6468,7 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B9" s="10">
         <v>2.0</v>
@@ -6448,10 +6477,10 @@
         <v>16.0</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G9" s="13">
         <f t="shared" ref="G9:G19" si="2">MULTIPLY(B9, C9)</f>
@@ -6460,7 +6489,7 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B10" s="10">
         <v>0.0</v>
@@ -6469,10 +6498,10 @@
         <v>10.0</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="2"/>
@@ -6481,7 +6510,7 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B11" s="10">
         <v>0.0</v>
@@ -6496,7 +6525,7 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="10">
         <v>4.0</v>
@@ -6511,7 +6540,7 @@
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10">
         <v>2.0</v>
@@ -6526,7 +6555,7 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B14" s="10">
         <v>1.0</v>
@@ -6541,7 +6570,7 @@
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B15" s="10">
         <v>4.0</v>
@@ -6550,7 +6579,7 @@
         <v>0.0</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" si="2"/>
@@ -6559,7 +6588,7 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B16" s="10">
         <v>1.0</v>
@@ -6574,7 +6603,7 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B17" s="10">
         <v>1.0</v>
@@ -6589,7 +6618,7 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B18" s="10">
         <v>2.0</v>
@@ -6604,7 +6633,7 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B19" s="10">
         <v>1.0</v>
@@ -6627,7 +6656,7 @@
     </row>
     <row r="22" ht="18.0" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -6660,7 +6689,7 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B23" s="10">
         <v>1.0</v>
@@ -6678,7 +6707,7 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B24" s="10">
         <v>1.0</v>
@@ -6693,7 +6722,7 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B25" s="10">
         <v>2.0</v>
@@ -6708,7 +6737,7 @@
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B26" s="10">
         <v>1.0</v>
@@ -6723,7 +6752,7 @@
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B27" s="10">
         <v>1.0</v>
@@ -6738,7 +6767,7 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B28" s="10">
         <v>1.0</v>
@@ -6757,7 +6786,7 @@
     </row>
     <row r="30" ht="18.0" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -6790,7 +6819,7 @@
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B31" s="10">
         <v>2.0</v>
@@ -6802,10 +6831,10 @@
         <v>8</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G31" s="13">
         <f t="shared" ref="G31:G32" si="4">MULTIPLY(B31, C31)</f>
@@ -6814,7 +6843,7 @@
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B32" s="10">
         <v>2.0</v>
@@ -6826,7 +6855,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G32" s="13">
         <f t="shared" si="4"/>
@@ -6849,7 +6878,7 @@
     </row>
     <row r="35" ht="18.0" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
@@ -6882,7 +6911,7 @@
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B36" s="10">
         <v>1.0</v>
@@ -6891,7 +6920,7 @@
         <v>80.0</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G36" s="13">
         <f t="shared" ref="G36:G38" si="5">MULTIPLY(B36, C36)</f>
@@ -6900,7 +6929,7 @@
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B37" s="10">
         <v>1.0</v>
@@ -6918,7 +6947,7 @@
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B38" s="10">
         <v>1.0</v>
@@ -6940,7 +6969,7 @@
     </row>
     <row r="40" ht="18.0" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -6973,7 +7002,7 @@
     </row>
     <row r="41">
       <c r="A41" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B41" s="10">
         <v>1.0</v>
@@ -6988,7 +7017,7 @@
     </row>
     <row r="42">
       <c r="A42" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B42" s="10">
         <v>1.0</v>
@@ -7003,7 +7032,7 @@
     </row>
     <row r="43">
       <c r="A43" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B43" s="10">
         <v>1.0</v>
@@ -7022,7 +7051,7 @@
     </row>
     <row r="45" ht="18.0" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
@@ -7055,7 +7084,7 @@
     </row>
     <row r="46">
       <c r="A46" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B46" s="10">
         <v>0.0</v>
@@ -7073,7 +7102,7 @@
     </row>
     <row r="47">
       <c r="A47" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B47" s="10">
         <v>3.0</v>
@@ -7085,10 +7114,10 @@
         <v>8</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G47" s="13">
         <f t="shared" si="7"/>

</xml_diff>